<commit_message>
Extracted movie info of new movies of 2016
</commit_message>
<xml_diff>
--- a/data/original_parkway_data/2016/Nightly Box Office Report (9).xlsx
+++ b/data/original_parkway_data/2016/Nightly Box Office Report (9).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="51917-052517" sheetId="1" state="visible" r:id="rId2"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="553">
   <si>
     <t xml:space="preserve">THE NEW PARKWAY THEATER</t>
   </si>
@@ -2709,7 +2709,7 @@
   <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3125,8 +3125,8 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="1" sqref="D9:K9 I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3652,7 +3652,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4188,7 +4188,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4720,7 +4720,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5256,7 +5256,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I27" activeCellId="1" sqref="D9:K9 I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5804,7 +5804,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="1" sqref="D9:K9 F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6328,8 +6328,8 @@
         <v>27</v>
       </c>
       <c r="I27" s="39" t="n">
-        <f aca="false">SUM(I7:I23)</f>
-        <v>12831</v>
+        <f aca="false">SUM(I7:I26)</f>
+        <v>14699</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6383,7 +6383,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="D9:K9 D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6762,7 +6762,9 @@
       </c>
       <c r="G19" s="42"/>
       <c r="H19" s="42"/>
-      <c r="I19" s="39"/>
+      <c r="I19" s="39" t="n">
+        <v>1370</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
@@ -6779,7 +6781,9 @@
         <v>449</v>
       </c>
       <c r="H20" s="42"/>
-      <c r="I20" s="39"/>
+      <c r="I20" s="39" t="n">
+        <v>987</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
@@ -6794,7 +6798,9 @@
       <c r="H21" s="42" t="n">
         <v>702</v>
       </c>
-      <c r="I21" s="39"/>
+      <c r="I21" s="39" t="n">
+        <v>702</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="33"/>
@@ -6809,7 +6815,7 @@
       </c>
       <c r="I22" s="39" t="n">
         <f aca="false">SUM(I7:I21)</f>
-        <v>11664</v>
+        <v>14723</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6846,7 +6852,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topRight" activeCell="C2" activeCellId="1" sqref="D9:K9 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7262,7 +7268,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7694,7 +7700,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8171,8 +8177,8 @@
   </sheetPr>
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8662,7 +8668,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E30" activeCellId="1" sqref="D9:K9 E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9143,7 +9149,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9608,7 +9614,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10125,7 +10131,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="D9:K9 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10677,7 +10683,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11150,7 +11156,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11624,7 +11630,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12103,7 +12109,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12574,7 +12580,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13072,7 +13078,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13553,13 +13559,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="1" sqref="D9:K9 D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.0491071428571"/>
   </cols>
@@ -13744,134 +13750,128 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="27" t="n">
-        <v>180</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B11" s="27"/>
       <c r="C11" s="27" t="n">
-        <v>568</v>
+        <v>54</v>
       </c>
       <c r="D11" s="27" t="n">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27" t="n">
-        <v>432</v>
-      </c>
-      <c r="H11" s="27"/>
+      <c r="F11" s="27" t="n">
+        <v>136</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="27" t="n">
+        <v>21</v>
+      </c>
       <c r="I11" s="28" t="n">
         <f aca="false">SUM(B11:H11)</f>
-        <v>1305</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="B12" s="27" t="n">
+        <v>316</v>
+      </c>
       <c r="C12" s="27" t="n">
-        <v>54</v>
+        <v>766</v>
       </c>
       <c r="D12" s="27" t="n">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="27" t="n">
-        <v>136</v>
-      </c>
-      <c r="G12" s="29"/>
+        <v>356</v>
+      </c>
+      <c r="G12" s="27" t="n">
+        <v>202</v>
+      </c>
       <c r="H12" s="27" t="n">
-        <v>21</v>
+        <v>318</v>
       </c>
       <c r="I12" s="28" t="n">
         <f aca="false">SUM(B12:H12)</f>
-        <v>371</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B13" s="27" t="n">
-        <v>316</v>
+        <v>12</v>
       </c>
       <c r="C13" s="27" t="n">
-        <v>766</v>
+        <v>0</v>
       </c>
       <c r="D13" s="27" t="n">
-        <v>180</v>
-      </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27" t="n">
-        <v>356</v>
-      </c>
-      <c r="G13" s="27" t="n">
-        <v>202</v>
-      </c>
-      <c r="H13" s="27" t="n">
-        <v>318</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E13" s="27" t="n">
+        <v>15</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
       <c r="I13" s="28" t="n">
         <f aca="false">SUM(B13:H13)</f>
-        <v>2138</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="27" t="n">
-        <v>12</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B14" s="27"/>
       <c r="C14" s="27" t="n">
-        <v>0</v>
+        <v>31.5</v>
       </c>
       <c r="D14" s="27" t="n">
-        <v>34</v>
-      </c>
-      <c r="E14" s="27" t="n">
-        <v>15</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="E14" s="27"/>
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="H14" s="27" t="n">
+        <v>142</v>
+      </c>
       <c r="I14" s="28" t="n">
         <f aca="false">SUM(B14:H14)</f>
-        <v>61</v>
+        <v>298.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27" t="n">
-        <v>31.5</v>
-      </c>
-      <c r="D15" s="27" t="n">
-        <v>125</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B15" s="27" t="n">
+        <v>386</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
-      <c r="H15" s="27" t="n">
-        <v>142</v>
-      </c>
+      <c r="H15" s="27"/>
       <c r="I15" s="28" t="n">
         <f aca="false">SUM(B15:H15)</f>
-        <v>298.5</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="27" t="n">
-        <v>386</v>
-      </c>
-      <c r="C16" s="27"/>
+        <v>50</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27" t="n">
+        <v>80</v>
+      </c>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
@@ -13879,61 +13879,57 @@
       <c r="H16" s="27"/>
       <c r="I16" s="28" t="n">
         <f aca="false">SUM(B16:H16)</f>
-        <v>386</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26" t="s">
-        <v>50</v>
+      <c r="A17" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="B17" s="27"/>
-      <c r="C17" s="27" t="n">
-        <v>80</v>
-      </c>
+      <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
+      <c r="F17" s="27" t="n">
+        <v>610</v>
+      </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
       <c r="I17" s="28" t="n">
         <f aca="false">SUM(B17:H17)</f>
-        <v>80</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="s">
-        <v>51</v>
+      <c r="A18" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
-      <c r="F18" s="27" t="n">
-        <v>610</v>
-      </c>
+      <c r="F18" s="27"/>
       <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="H18" s="27" t="n">
+        <v>158</v>
+      </c>
       <c r="I18" s="28" t="n">
         <f aca="false">SUM(B18:H18)</f>
-        <v>610</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="s">
-        <v>52</v>
-      </c>
+      <c r="A19" s="30"/>
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27" t="n">
-        <v>158</v>
-      </c>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
       <c r="I19" s="28" t="n">
         <f aca="false">SUM(B19:H19)</f>
-        <v>158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14021,47 +14017,33 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="28" t="n">
-        <f aca="false">SUM(B26:H26)</f>
-        <v>0</v>
+      <c r="A26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="28" t="e">
+        <f aca="false">SUM(I7:I22)E21</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="33"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="28" t="n">
-        <f aca="false">SUM(I7:I23)</f>
-        <v>7268.5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36" t="s">
+      <c r="A27" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="22"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14082,7 +14064,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="1" sqref="D9:K9 I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14596,7 +14578,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15103,7 +15085,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15604,7 +15586,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="1" sqref="D9:K9 A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16080,7 +16062,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16534,7 +16516,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17010,7 +16992,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17560,7 +17542,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="1" sqref="D9:K9 F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18042,7 +18024,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18539,7 +18521,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19038,7 +19020,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19564,7 +19546,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20069,7 +20051,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20558,7 +20540,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21091,7 +21073,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="1" sqref="D9:K9 I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21583,7 +21565,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22094,7 +22076,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22117,7 +22099,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22623,7 +22605,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23124,7 +23106,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23649,7 +23631,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24152,7 +24134,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24673,7 +24655,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25158,7 +25140,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26029,7 +26011,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26522,7 +26504,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27047,7 +27029,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27545,7 +27527,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -27568,7 +27550,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28090,7 +28072,7 @@
   <dimension ref="A2:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28637,7 +28619,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29189,7 +29171,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D9:K9 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>